<commit_message>
bug fix on list filter from mans and prods
</commit_message>
<xml_diff>
--- a/SpeCalcCode/SpeCalc/obj/Release/AspnetCompileMerge/Source/App_Data/Specification_fin.xlsx
+++ b/SpeCalcCode/SpeCalc/obj/Release/AspnetCompileMerge/Source/App_Data/Specification_fin.xlsx
@@ -15,18 +15,18 @@
     <sheet name="WorkSheet" sheetId="19" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">WorkSheet!$A$15:$N$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">WorkSheet!$A$15:$O$22</definedName>
     <definedName name="OLE_LINK1" localSheetId="0">WorkSheet!#REF!</definedName>
     <definedName name="OLE_LINK3" localSheetId="0">WorkSheet!#REF!</definedName>
     <definedName name="OLE_LINK5" localSheetId="0">WorkSheet!#REF!</definedName>
-    <definedName name="USD">WorkSheet!$D$1</definedName>
+    <definedName name="USD">WorkSheet!$E$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Курс Доллара</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Курс Евро</t>
   </si>
   <si>
-    <t>Каталожный номер</t>
-  </si>
-  <si>
     <t>Цена, $ от снаб.</t>
   </si>
   <si>
@@ -125,25 +122,40 @@
   </si>
   <si>
     <t>Комментарий</t>
+  </si>
+  <si>
+    <t>Каталожный № (запрос)</t>
+  </si>
+  <si>
+    <t>Каталожный № (ответ)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="#,##0&quot;р.&quot;"/>
     <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="167" formatCode="#,##0.00_р_."/>
     <numFmt numFmtId="168" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="176" formatCode="\₽\ #,##0.00"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial Cyr"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -320,190 +332,201 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="24">
     <cellStyle name="Normal_AVAYA" xfId="7"/>
     <cellStyle name="Гиперссылка 2" xfId="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -518,11 +541,16 @@
     <cellStyle name="Обычный 4 2" xfId="14"/>
     <cellStyle name="Обычный 4 2 2" xfId="15"/>
     <cellStyle name="Обычный 5" xfId="5"/>
+    <cellStyle name="Обычный 5 2" xfId="20"/>
     <cellStyle name="Обычный 6" xfId="16"/>
+    <cellStyle name="Обычный 7" xfId="23"/>
     <cellStyle name="Процентный 2" xfId="4"/>
+    <cellStyle name="Процентный 2 2" xfId="19"/>
     <cellStyle name="Стиль 1" xfId="17"/>
     <cellStyle name="Финансовый 10" xfId="18"/>
+    <cellStyle name="Финансовый 10 2" xfId="22"/>
     <cellStyle name="Финансовый 2" xfId="6"/>
+    <cellStyle name="Финансовый 2 2" xfId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -833,72 +861,73 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W55"/>
+  <dimension ref="A1:X55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="15" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="45.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" style="38" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="19.5703125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="20.28515625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="23.85546875" style="4" customWidth="1"/>
-    <col min="17" max="18" width="18.42578125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="25.28515625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="45.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="1"/>
-    <col min="22" max="22" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" style="1"/>
-    <col min="24" max="24" width="19.140625" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="30.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" style="38" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="19.5703125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="20.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="23.85546875" style="4" customWidth="1"/>
+    <col min="18" max="19" width="18.42578125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="25.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="45.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" style="1"/>
+    <col min="23" max="23" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="1"/>
+    <col min="25" max="25" width="19.140625" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="37"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="D1" s="41"/>
+      <c r="E1" s="37"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C2" s="41" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="37"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C3" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="37"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="C4" s="47" t="s">
         <v>27</v>
-      </c>
-      <c r="D3" s="37"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C4" s="47" t="s">
-        <v>28</v>
       </c>
       <c r="D4" s="37">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="39" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="22"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -908,24 +937,24 @@
       <c r="L5" s="22"/>
       <c r="M5" s="22"/>
       <c r="N5" s="22"/>
-      <c r="O5" s="12"/>
+      <c r="O5" s="22"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
-      <c r="S5" s="17"/>
+      <c r="S5" s="12"/>
       <c r="T5" s="17"/>
       <c r="U5" s="17"/>
       <c r="V5" s="17"/>
       <c r="W5" s="17"/>
-    </row>
-    <row r="6" spans="1:23" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="X5" s="17"/>
+    </row>
+    <row r="6" spans="1:24" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="39" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="51"/>
       <c r="F6" s="51"/>
       <c r="G6" s="51"/>
       <c r="H6" s="51"/>
@@ -935,24 +964,24 @@
       <c r="L6" s="51"/>
       <c r="M6" s="51"/>
       <c r="N6" s="51"/>
-      <c r="O6" s="12"/>
+      <c r="O6" s="51"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
-      <c r="S6" s="17"/>
+      <c r="S6" s="12"/>
       <c r="T6" s="17"/>
       <c r="U6" s="17"/>
       <c r="V6" s="17"/>
       <c r="W6" s="17"/>
-    </row>
-    <row r="7" spans="1:23" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="X6" s="17"/>
+    </row>
+    <row r="7" spans="1:24" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="39" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="51"/>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
       <c r="H7" s="51"/>
@@ -962,24 +991,24 @@
       <c r="L7" s="51"/>
       <c r="M7" s="51"/>
       <c r="N7" s="51"/>
-      <c r="O7" s="12"/>
+      <c r="O7" s="51"/>
       <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
-      <c r="S7" s="17"/>
+      <c r="S7" s="12"/>
       <c r="T7" s="17"/>
       <c r="U7" s="17"/>
       <c r="V7" s="17"/>
       <c r="W7" s="17"/>
-    </row>
-    <row r="8" spans="1:23" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="X7" s="17"/>
+    </row>
+    <row r="8" spans="1:24" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="40" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="52"/>
       <c r="F8" s="52"/>
       <c r="G8" s="52"/>
       <c r="H8" s="52"/>
@@ -989,24 +1018,24 @@
       <c r="L8" s="52"/>
       <c r="M8" s="52"/>
       <c r="N8" s="52"/>
-      <c r="O8" s="13"/>
+      <c r="O8" s="52"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
       <c r="R8" s="13"/>
-      <c r="S8" s="17"/>
+      <c r="S8" s="13"/>
       <c r="T8" s="17"/>
       <c r="U8" s="17"/>
       <c r="V8" s="17"/>
       <c r="W8" s="17"/>
-    </row>
-    <row r="9" spans="1:23" s="5" customFormat="1" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="X8" s="17"/>
+    </row>
+    <row r="9" spans="1:24" s="5" customFormat="1" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="41" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="11"/>
-      <c r="E9" s="50"/>
       <c r="F9" s="50"/>
       <c r="G9" s="50"/>
       <c r="H9" s="50"/>
@@ -1016,19 +1045,19 @@
       <c r="L9" s="50"/>
       <c r="M9" s="50"/>
       <c r="N9" s="50"/>
-      <c r="O9" s="16"/>
+      <c r="O9" s="50"/>
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
-    </row>
-    <row r="10" spans="1:23" s="5" customFormat="1" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="S9" s="16"/>
+    </row>
+    <row r="10" spans="1:24" s="5" customFormat="1" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="48"/>
       <c r="F10" s="48"/>
       <c r="G10" s="48"/>
       <c r="H10" s="48"/>
@@ -1038,19 +1067,19 @@
       <c r="L10" s="48"/>
       <c r="M10" s="48"/>
       <c r="N10" s="48"/>
-      <c r="O10" s="14"/>
+      <c r="O10" s="48"/>
       <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
       <c r="R10" s="14"/>
-    </row>
-    <row r="11" spans="1:23" s="5" customFormat="1" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="S10" s="14"/>
+    </row>
+    <row r="11" spans="1:24" s="5" customFormat="1" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="41" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="49"/>
       <c r="F11" s="49"/>
       <c r="G11" s="49"/>
       <c r="H11" s="49"/>
@@ -1060,19 +1089,19 @@
       <c r="L11" s="49"/>
       <c r="M11" s="49"/>
       <c r="N11" s="49"/>
-      <c r="O11" s="15"/>
+      <c r="O11" s="49"/>
       <c r="P11" s="15"/>
       <c r="Q11" s="15"/>
       <c r="R11" s="15"/>
-    </row>
-    <row r="12" spans="1:23" s="5" customFormat="1" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="S11" s="15"/>
+    </row>
+    <row r="12" spans="1:24" s="5" customFormat="1" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="41" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="9"/>
-      <c r="E12" s="51"/>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
       <c r="H12" s="51"/>
@@ -1082,19 +1111,19 @@
       <c r="L12" s="51"/>
       <c r="M12" s="51"/>
       <c r="N12" s="51"/>
-      <c r="O12" s="12"/>
+      <c r="O12" s="51"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
       <c r="R12" s="12"/>
-    </row>
-    <row r="13" spans="1:23" s="5" customFormat="1" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="S12" s="12"/>
+    </row>
+    <row r="13" spans="1:24" s="5" customFormat="1" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="41" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="10"/>
-      <c r="E13" s="48"/>
       <c r="F13" s="48"/>
       <c r="G13" s="48"/>
       <c r="H13" s="48"/>
@@ -1104,486 +1133,509 @@
       <c r="L13" s="48"/>
       <c r="M13" s="48"/>
       <c r="N13" s="48"/>
-      <c r="O13" s="14"/>
+      <c r="O13" s="48"/>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
       <c r="R13" s="14"/>
-    </row>
-    <row r="14" spans="1:23" s="5" customFormat="1" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="S13" s="14"/>
+    </row>
+    <row r="14" spans="1:24" s="5" customFormat="1" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="42" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="20"/>
-      <c r="O14" s="15"/>
       <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
       <c r="R14" s="15"/>
-    </row>
-    <row r="15" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="S14" s="15"/>
+    </row>
+    <row r="15" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="18" t="s">
+      <c r="L15" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="M15" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="P15" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q15" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="R15" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="S15" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="T15" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="U15" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="L15" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="M15" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="N15" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="O15" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="P15" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q15" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="R15" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="S15" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="T15" s="19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:24" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="27"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="44"/>
       <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
+      <c r="G16" s="27"/>
       <c r="H16" s="28"/>
       <c r="I16" s="28"/>
-      <c r="J16" s="29"/>
+      <c r="J16" s="28"/>
       <c r="K16" s="29"/>
       <c r="L16" s="29"/>
-      <c r="M16" s="30"/>
+      <c r="M16" s="29"/>
       <c r="N16" s="30"/>
       <c r="O16" s="30"/>
       <c r="P16" s="30"/>
       <c r="Q16" s="30"/>
       <c r="R16" s="30"/>
-      <c r="S16" s="23"/>
-    </row>
-    <row r="17" spans="1:19" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="S16" s="30"/>
+      <c r="T16" s="23"/>
+    </row>
+    <row r="17" spans="1:20" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="27"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="44"/>
       <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
-      <c r="J17" s="29"/>
+      <c r="J17" s="28"/>
       <c r="K17" s="29"/>
       <c r="L17" s="29"/>
-      <c r="M17" s="30"/>
+      <c r="M17" s="29"/>
       <c r="N17" s="30"/>
       <c r="O17" s="30"/>
       <c r="P17" s="30"/>
       <c r="Q17" s="30"/>
       <c r="R17" s="30"/>
-      <c r="S17" s="23"/>
-    </row>
-    <row r="18" spans="1:19" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="S17" s="30"/>
+      <c r="T17" s="23"/>
+    </row>
+    <row r="18" spans="1:20" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="27"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="44"/>
       <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
+      <c r="G18" s="27"/>
       <c r="H18" s="28"/>
       <c r="I18" s="28"/>
-      <c r="J18" s="29"/>
+      <c r="J18" s="28"/>
       <c r="K18" s="29"/>
       <c r="L18" s="29"/>
-      <c r="M18" s="30"/>
+      <c r="M18" s="29"/>
       <c r="N18" s="30"/>
       <c r="O18" s="30"/>
       <c r="P18" s="30"/>
       <c r="Q18" s="30"/>
       <c r="R18" s="30"/>
-      <c r="S18" s="23"/>
-    </row>
-    <row r="19" spans="1:19" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="S18" s="30"/>
+      <c r="T18" s="23"/>
+    </row>
+    <row r="19" spans="1:20" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="26"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="27"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="45"/>
       <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
+      <c r="G19" s="27"/>
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
       <c r="J19" s="28"/>
       <c r="K19" s="28"/>
       <c r="L19" s="28"/>
-      <c r="M19" s="30"/>
+      <c r="M19" s="28"/>
       <c r="N19" s="30"/>
       <c r="O19" s="30"/>
       <c r="P19" s="30"/>
       <c r="Q19" s="30"/>
       <c r="R19" s="30"/>
-      <c r="S19" s="23"/>
-    </row>
-    <row r="20" spans="1:19" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="S19" s="30"/>
+      <c r="T19" s="23"/>
+    </row>
+    <row r="20" spans="1:20" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="27"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="44"/>
       <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
+      <c r="G20" s="27"/>
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
       <c r="J20" s="28"/>
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
-      <c r="M20" s="30"/>
+      <c r="M20" s="28"/>
       <c r="N20" s="30"/>
       <c r="O20" s="30"/>
       <c r="P20" s="30"/>
       <c r="Q20" s="30"/>
       <c r="R20" s="30"/>
-      <c r="S20" s="23"/>
-    </row>
-    <row r="21" spans="1:19" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="S20" s="30"/>
+      <c r="T20" s="23"/>
+    </row>
+    <row r="21" spans="1:20" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="26"/>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="27"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="45"/>
       <c r="F21" s="27"/>
-      <c r="G21" s="32"/>
+      <c r="G21" s="27"/>
       <c r="H21" s="32"/>
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
       <c r="L21" s="32"/>
-      <c r="M21" s="30"/>
+      <c r="M21" s="32"/>
       <c r="N21" s="30"/>
       <c r="O21" s="30"/>
       <c r="P21" s="30"/>
       <c r="Q21" s="30"/>
       <c r="R21" s="30"/>
-      <c r="S21" s="24"/>
-    </row>
-    <row r="22" spans="1:19" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="S21" s="30"/>
+      <c r="T21" s="24"/>
+    </row>
+    <row r="22" spans="1:20" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="26"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="27"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="45"/>
       <c r="F22" s="27"/>
-      <c r="G22" s="32"/>
+      <c r="G22" s="27"/>
       <c r="H22" s="32"/>
       <c r="I22" s="32"/>
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
       <c r="L22" s="32"/>
-      <c r="M22" s="30"/>
+      <c r="M22" s="32"/>
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
       <c r="P22" s="30"/>
       <c r="Q22" s="30"/>
       <c r="R22" s="30"/>
-      <c r="S22" s="24"/>
-    </row>
-    <row r="23" spans="1:19" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="S22" s="30"/>
+      <c r="T22" s="24"/>
+    </row>
+    <row r="23" spans="1:20" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="26"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="27"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="45"/>
       <c r="F23" s="27"/>
-      <c r="G23" s="32"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="32"/>
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
       <c r="L23" s="32"/>
-      <c r="M23" s="30"/>
+      <c r="M23" s="32"/>
       <c r="N23" s="30"/>
       <c r="O23" s="30"/>
       <c r="P23" s="30"/>
       <c r="Q23" s="30"/>
       <c r="R23" s="30"/>
-      <c r="S23" s="24"/>
-    </row>
-    <row r="24" spans="1:19" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="S23" s="30"/>
+      <c r="T23" s="24"/>
+    </row>
+    <row r="24" spans="1:20" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="26"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="27"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="45"/>
       <c r="F24" s="27"/>
-      <c r="G24" s="32"/>
+      <c r="G24" s="27"/>
       <c r="H24" s="32"/>
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
       <c r="L24" s="32"/>
-      <c r="M24" s="30"/>
+      <c r="M24" s="32"/>
       <c r="N24" s="30"/>
       <c r="O24" s="30"/>
       <c r="P24" s="30"/>
       <c r="Q24" s="30"/>
       <c r="R24" s="30"/>
-      <c r="S24" s="24"/>
-    </row>
-    <row r="25" spans="1:19" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="S24" s="30"/>
+      <c r="T24" s="24"/>
+    </row>
+    <row r="25" spans="1:20" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="26"/>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="27"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="45"/>
       <c r="F25" s="27"/>
-      <c r="G25" s="32"/>
+      <c r="G25" s="27"/>
       <c r="H25" s="32"/>
       <c r="I25" s="32"/>
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
       <c r="L25" s="32"/>
-      <c r="M25" s="30"/>
+      <c r="M25" s="32"/>
       <c r="N25" s="30"/>
       <c r="O25" s="30"/>
       <c r="P25" s="30"/>
       <c r="Q25" s="30"/>
       <c r="R25" s="30"/>
-      <c r="S25" s="24"/>
-    </row>
-    <row r="26" spans="1:19" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="S25" s="30"/>
+      <c r="T25" s="24"/>
+    </row>
+    <row r="26" spans="1:20" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="26"/>
       <c r="B26" s="26"/>
       <c r="C26" s="26"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="27"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="45"/>
       <c r="F26" s="27"/>
-      <c r="G26" s="33"/>
+      <c r="G26" s="27"/>
       <c r="H26" s="33"/>
       <c r="I26" s="33"/>
       <c r="J26" s="33"/>
       <c r="K26" s="33"/>
       <c r="L26" s="33"/>
-      <c r="M26" s="30"/>
+      <c r="M26" s="33"/>
       <c r="N26" s="30"/>
       <c r="O26" s="30"/>
       <c r="P26" s="30"/>
       <c r="Q26" s="30"/>
       <c r="R26" s="30"/>
-      <c r="S26" s="24"/>
-    </row>
-    <row r="27" spans="1:19" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="S26" s="30"/>
+      <c r="T26" s="24"/>
+    </row>
+    <row r="27" spans="1:20" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="26"/>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="27"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="45"/>
       <c r="F27" s="27"/>
-      <c r="G27" s="33"/>
+      <c r="G27" s="27"/>
       <c r="H27" s="33"/>
       <c r="I27" s="33"/>
       <c r="J27" s="33"/>
       <c r="K27" s="33"/>
       <c r="L27" s="33"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="34"/>
       <c r="O27" s="33"/>
       <c r="P27" s="33"/>
       <c r="Q27" s="33"/>
-      <c r="R27" s="35"/>
-      <c r="S27" s="24"/>
-    </row>
-    <row r="28" spans="1:19" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="R27" s="33"/>
+      <c r="S27" s="35"/>
+      <c r="T27" s="24"/>
+    </row>
+    <row r="28" spans="1:20" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="26"/>
       <c r="B28" s="26"/>
       <c r="C28" s="26"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="27"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="45"/>
       <c r="F28" s="27"/>
-      <c r="G28" s="34"/>
+      <c r="G28" s="27"/>
       <c r="H28" s="34"/>
       <c r="I28" s="34"/>
-      <c r="J28" s="33"/>
+      <c r="J28" s="34"/>
       <c r="K28" s="33"/>
       <c r="L28" s="33"/>
-      <c r="M28" s="34"/>
+      <c r="M28" s="33"/>
       <c r="N28" s="34"/>
       <c r="O28" s="34"/>
       <c r="P28" s="34"/>
       <c r="Q28" s="34"/>
       <c r="R28" s="34"/>
-      <c r="S28" s="24"/>
-    </row>
-    <row r="29" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S28" s="34"/>
+      <c r="T28" s="24"/>
+    </row>
+    <row r="29" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="26"/>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="27"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="45"/>
       <c r="F29" s="27"/>
-      <c r="G29" s="21"/>
+      <c r="G29" s="27"/>
       <c r="H29" s="21"/>
       <c r="I29" s="21"/>
-      <c r="J29" s="32"/>
+      <c r="J29" s="21"/>
       <c r="K29" s="32"/>
       <c r="L29" s="32"/>
-      <c r="M29" s="21"/>
+      <c r="M29" s="32"/>
       <c r="N29" s="21"/>
       <c r="O29" s="21"/>
       <c r="P29" s="21"/>
       <c r="Q29" s="21"/>
       <c r="R29" s="21"/>
-    </row>
-    <row r="30" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S29" s="21"/>
+    </row>
+    <row r="30" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="26"/>
       <c r="B30" s="26"/>
       <c r="C30" s="26"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="27"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="45"/>
       <c r="F30" s="27"/>
-      <c r="G30" s="21"/>
+      <c r="G30" s="27"/>
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
-      <c r="J30" s="32"/>
+      <c r="J30" s="21"/>
       <c r="K30" s="32"/>
       <c r="L30" s="32"/>
-      <c r="M30" s="21"/>
+      <c r="M30" s="32"/>
       <c r="N30" s="21"/>
       <c r="O30" s="21"/>
       <c r="P30" s="21"/>
       <c r="Q30" s="21"/>
       <c r="R30" s="21"/>
-    </row>
-    <row r="31" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S30" s="21"/>
+    </row>
+    <row r="31" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="26"/>
       <c r="B31" s="26"/>
       <c r="C31" s="26"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="27"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="45"/>
       <c r="F31" s="27"/>
-      <c r="G31" s="21"/>
+      <c r="G31" s="27"/>
       <c r="H31" s="21"/>
       <c r="I31" s="21"/>
-      <c r="J31" s="32"/>
+      <c r="J31" s="21"/>
       <c r="K31" s="32"/>
       <c r="L31" s="32"/>
-      <c r="M31" s="21"/>
+      <c r="M31" s="32"/>
       <c r="N31" s="21"/>
       <c r="O31" s="21"/>
       <c r="P31" s="21"/>
       <c r="Q31" s="21"/>
       <c r="R31" s="21"/>
-    </row>
-    <row r="32" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S31" s="21"/>
+    </row>
+    <row r="32" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="26"/>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="27"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="45"/>
       <c r="F32" s="27"/>
-      <c r="G32" s="21"/>
+      <c r="G32" s="27"/>
       <c r="H32" s="21"/>
       <c r="I32" s="21"/>
-      <c r="J32" s="32"/>
+      <c r="J32" s="21"/>
       <c r="K32" s="32"/>
       <c r="L32" s="32"/>
-      <c r="M32" s="21"/>
+      <c r="M32" s="32"/>
       <c r="N32" s="21"/>
       <c r="O32" s="21"/>
       <c r="P32" s="21"/>
       <c r="Q32" s="21"/>
       <c r="R32" s="21"/>
-    </row>
-    <row r="33" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S32" s="21"/>
+    </row>
+    <row r="33" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="26"/>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="27"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="45"/>
       <c r="F33" s="27"/>
-      <c r="G33" s="21"/>
+      <c r="G33" s="27"/>
       <c r="H33" s="21"/>
       <c r="I33" s="21"/>
-      <c r="J33" s="32"/>
+      <c r="J33" s="21"/>
       <c r="K33" s="32"/>
       <c r="L33" s="32"/>
-      <c r="M33" s="21"/>
+      <c r="M33" s="32"/>
       <c r="N33" s="21"/>
       <c r="O33" s="21"/>
       <c r="P33" s="21"/>
       <c r="Q33" s="21"/>
       <c r="R33" s="21"/>
-    </row>
-    <row r="34" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S33" s="21"/>
+    </row>
+    <row r="34" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="26"/>
       <c r="B34" s="26"/>
       <c r="C34" s="26"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="27"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="45"/>
       <c r="F34" s="27"/>
-      <c r="G34" s="21"/>
+      <c r="G34" s="27"/>
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
-      <c r="J34" s="32"/>
+      <c r="J34" s="21"/>
       <c r="K34" s="32"/>
       <c r="L34" s="32"/>
-      <c r="M34" s="21"/>
+      <c r="M34" s="32"/>
       <c r="N34" s="21"/>
       <c r="O34" s="21"/>
       <c r="P34" s="21"/>
       <c r="Q34" s="21"/>
       <c r="R34" s="21"/>
-    </row>
-    <row r="35" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S34" s="21"/>
+    </row>
+    <row r="35" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="26"/>
       <c r="B35" s="26"/>
       <c r="C35" s="26"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="27"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="45"/>
       <c r="F35" s="27"/>
-      <c r="G35" s="21"/>
+      <c r="G35" s="27"/>
       <c r="H35" s="21"/>
       <c r="I35" s="21"/>
       <c r="J35" s="21"/>
@@ -1595,15 +1647,16 @@
       <c r="P35" s="21"/>
       <c r="Q35" s="21"/>
       <c r="R35" s="21"/>
-    </row>
-    <row r="36" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S35" s="21"/>
+    </row>
+    <row r="36" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="26"/>
       <c r="B36" s="26"/>
       <c r="C36" s="26"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="27"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="45"/>
       <c r="F36" s="27"/>
-      <c r="G36" s="21"/>
+      <c r="G36" s="27"/>
       <c r="H36" s="21"/>
       <c r="I36" s="21"/>
       <c r="J36" s="21"/>
@@ -1615,15 +1668,16 @@
       <c r="P36" s="21"/>
       <c r="Q36" s="21"/>
       <c r="R36" s="21"/>
-    </row>
-    <row r="37" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S36" s="21"/>
+    </row>
+    <row r="37" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="26"/>
       <c r="B37" s="26"/>
       <c r="C37" s="26"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="27"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="45"/>
       <c r="F37" s="27"/>
-      <c r="G37" s="21"/>
+      <c r="G37" s="27"/>
       <c r="H37" s="21"/>
       <c r="I37" s="21"/>
       <c r="J37" s="21"/>
@@ -1635,15 +1689,16 @@
       <c r="P37" s="21"/>
       <c r="Q37" s="21"/>
       <c r="R37" s="21"/>
-    </row>
-    <row r="38" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S37" s="21"/>
+    </row>
+    <row r="38" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="26"/>
       <c r="B38" s="26"/>
       <c r="C38" s="26"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="27"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="45"/>
       <c r="F38" s="27"/>
-      <c r="G38" s="21"/>
+      <c r="G38" s="27"/>
       <c r="H38" s="21"/>
       <c r="I38" s="21"/>
       <c r="J38" s="21"/>
@@ -1655,15 +1710,16 @@
       <c r="P38" s="21"/>
       <c r="Q38" s="21"/>
       <c r="R38" s="21"/>
-    </row>
-    <row r="39" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S38" s="21"/>
+    </row>
+    <row r="39" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="27"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="45"/>
       <c r="F39" s="27"/>
-      <c r="G39" s="21"/>
+      <c r="G39" s="27"/>
       <c r="H39" s="21"/>
       <c r="I39" s="21"/>
       <c r="J39" s="21"/>
@@ -1675,15 +1731,16 @@
       <c r="P39" s="21"/>
       <c r="Q39" s="21"/>
       <c r="R39" s="21"/>
-    </row>
-    <row r="40" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S39" s="21"/>
+    </row>
+    <row r="40" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="26"/>
       <c r="B40" s="26"/>
       <c r="C40" s="26"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="27"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="45"/>
       <c r="F40" s="27"/>
-      <c r="G40" s="21"/>
+      <c r="G40" s="27"/>
       <c r="H40" s="21"/>
       <c r="I40" s="21"/>
       <c r="J40" s="21"/>
@@ -1695,15 +1752,16 @@
       <c r="P40" s="21"/>
       <c r="Q40" s="21"/>
       <c r="R40" s="21"/>
-    </row>
-    <row r="41" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S40" s="21"/>
+    </row>
+    <row r="41" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="26"/>
       <c r="B41" s="26"/>
       <c r="C41" s="26"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="27"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="45"/>
       <c r="F41" s="27"/>
-      <c r="G41" s="21"/>
+      <c r="G41" s="27"/>
       <c r="H41" s="21"/>
       <c r="I41" s="21"/>
       <c r="J41" s="21"/>
@@ -1715,15 +1773,16 @@
       <c r="P41" s="21"/>
       <c r="Q41" s="21"/>
       <c r="R41" s="21"/>
-    </row>
-    <row r="42" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S41" s="21"/>
+    </row>
+    <row r="42" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="26"/>
       <c r="B42" s="26"/>
       <c r="C42" s="26"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="27"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="45"/>
       <c r="F42" s="27"/>
-      <c r="G42" s="21"/>
+      <c r="G42" s="27"/>
       <c r="H42" s="21"/>
       <c r="I42" s="21"/>
       <c r="J42" s="21"/>
@@ -1735,15 +1794,16 @@
       <c r="P42" s="21"/>
       <c r="Q42" s="21"/>
       <c r="R42" s="21"/>
-    </row>
-    <row r="43" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S42" s="21"/>
+    </row>
+    <row r="43" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="26"/>
       <c r="B43" s="26"/>
       <c r="C43" s="26"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="27"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="45"/>
       <c r="F43" s="27"/>
-      <c r="G43" s="21"/>
+      <c r="G43" s="27"/>
       <c r="H43" s="21"/>
       <c r="I43" s="21"/>
       <c r="J43" s="21"/>
@@ -1755,15 +1815,16 @@
       <c r="P43" s="21"/>
       <c r="Q43" s="21"/>
       <c r="R43" s="21"/>
-    </row>
-    <row r="44" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S43" s="21"/>
+    </row>
+    <row r="44" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="21"/>
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="27"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="45"/>
       <c r="F44" s="27"/>
-      <c r="G44" s="21"/>
+      <c r="G44" s="27"/>
       <c r="H44" s="21"/>
       <c r="I44" s="21"/>
       <c r="J44" s="21"/>
@@ -1775,15 +1836,16 @@
       <c r="P44" s="21"/>
       <c r="Q44" s="21"/>
       <c r="R44" s="21"/>
-    </row>
-    <row r="45" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S44" s="21"/>
+    </row>
+    <row r="45" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="21"/>
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="27"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="45"/>
       <c r="F45" s="27"/>
-      <c r="G45" s="21"/>
+      <c r="G45" s="27"/>
       <c r="H45" s="21"/>
       <c r="I45" s="21"/>
       <c r="J45" s="21"/>
@@ -1795,15 +1857,16 @@
       <c r="P45" s="21"/>
       <c r="Q45" s="21"/>
       <c r="R45" s="21"/>
-    </row>
-    <row r="46" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S45" s="21"/>
+    </row>
+    <row r="46" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="21"/>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="27"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="45"/>
       <c r="F46" s="27"/>
-      <c r="G46" s="21"/>
+      <c r="G46" s="27"/>
       <c r="H46" s="21"/>
       <c r="I46" s="21"/>
       <c r="J46" s="21"/>
@@ -1815,15 +1878,16 @@
       <c r="P46" s="21"/>
       <c r="Q46" s="21"/>
       <c r="R46" s="21"/>
-    </row>
-    <row r="47" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S46" s="21"/>
+    </row>
+    <row r="47" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="21"/>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="32"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="21"/>
       <c r="H47" s="32"/>
       <c r="I47" s="32"/>
       <c r="J47" s="32"/>
@@ -1835,15 +1899,16 @@
       <c r="P47" s="32"/>
       <c r="Q47" s="32"/>
       <c r="R47" s="32"/>
-    </row>
-    <row r="48" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S47" s="32"/>
+    </row>
+    <row r="48" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="21"/>
       <c r="B48" s="21"/>
       <c r="C48" s="21"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="32"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="21"/>
       <c r="H48" s="32"/>
       <c r="I48" s="32"/>
       <c r="J48" s="32"/>
@@ -1855,15 +1920,16 @@
       <c r="P48" s="32"/>
       <c r="Q48" s="32"/>
       <c r="R48" s="32"/>
-    </row>
-    <row r="49" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S48" s="32"/>
+    </row>
+    <row r="49" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="21"/>
       <c r="B49" s="21"/>
       <c r="C49" s="21"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="36"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="32"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="21"/>
       <c r="H49" s="32"/>
       <c r="I49" s="32"/>
       <c r="J49" s="32"/>
@@ -1875,15 +1941,16 @@
       <c r="P49" s="32"/>
       <c r="Q49" s="32"/>
       <c r="R49" s="32"/>
-    </row>
-    <row r="50" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S49" s="32"/>
+    </row>
+    <row r="50" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="21"/>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="32"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="21"/>
       <c r="H50" s="32"/>
       <c r="I50" s="32"/>
       <c r="J50" s="32"/>
@@ -1895,15 +1962,16 @@
       <c r="P50" s="32"/>
       <c r="Q50" s="32"/>
       <c r="R50" s="32"/>
-    </row>
-    <row r="51" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S50" s="32"/>
+    </row>
+    <row r="51" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="26"/>
       <c r="B51" s="26"/>
       <c r="C51" s="26"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="32"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="36"/>
+      <c r="G51" s="21"/>
       <c r="H51" s="32"/>
       <c r="I51" s="32"/>
       <c r="J51" s="32"/>
@@ -1915,15 +1983,16 @@
       <c r="P51" s="32"/>
       <c r="Q51" s="32"/>
       <c r="R51" s="32"/>
-    </row>
-    <row r="52" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S51" s="32"/>
+    </row>
+    <row r="52" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="26"/>
       <c r="B52" s="26"/>
       <c r="C52" s="26"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="32"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="36"/>
+      <c r="G52" s="21"/>
       <c r="H52" s="32"/>
       <c r="I52" s="32"/>
       <c r="J52" s="32"/>
@@ -1935,15 +2004,16 @@
       <c r="P52" s="32"/>
       <c r="Q52" s="32"/>
       <c r="R52" s="32"/>
-    </row>
-    <row r="53" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S52" s="32"/>
+    </row>
+    <row r="53" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="26"/>
       <c r="B53" s="26"/>
       <c r="C53" s="26"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="32"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="45"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="21"/>
       <c r="H53" s="32"/>
       <c r="I53" s="32"/>
       <c r="J53" s="32"/>
@@ -1955,15 +2025,16 @@
       <c r="P53" s="32"/>
       <c r="Q53" s="32"/>
       <c r="R53" s="32"/>
-    </row>
-    <row r="54" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S53" s="32"/>
+    </row>
+    <row r="54" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="21"/>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="32"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="36"/>
+      <c r="G54" s="21"/>
       <c r="H54" s="32"/>
       <c r="I54" s="32"/>
       <c r="J54" s="32"/>
@@ -1975,15 +2046,16 @@
       <c r="P54" s="32"/>
       <c r="Q54" s="32"/>
       <c r="R54" s="32"/>
-    </row>
-    <row r="55" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S54" s="32"/>
+    </row>
+    <row r="55" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="21"/>
-      <c r="D55" s="46"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="21"/>
-      <c r="G55" s="32"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="36"/>
+      <c r="G55" s="21"/>
       <c r="H55" s="32"/>
       <c r="I55" s="32"/>
       <c r="J55" s="32"/>
@@ -1995,18 +2067,19 @@
       <c r="P55" s="32"/>
       <c r="Q55" s="32"/>
       <c r="R55" s="32"/>
+      <c r="S55" s="32"/>
     </row>
   </sheetData>
-  <autoFilter ref="A15:N22"/>
+  <autoFilter ref="A15:O22"/>
   <mergeCells count="8">
-    <mergeCell ref="E13:N13"/>
-    <mergeCell ref="E10:N10"/>
-    <mergeCell ref="E11:N11"/>
-    <mergeCell ref="E9:N9"/>
-    <mergeCell ref="E6:N6"/>
-    <mergeCell ref="E7:N7"/>
-    <mergeCell ref="E12:N12"/>
-    <mergeCell ref="E8:N8"/>
+    <mergeCell ref="F13:O13"/>
+    <mergeCell ref="F10:O10"/>
+    <mergeCell ref="F11:O11"/>
+    <mergeCell ref="F9:O9"/>
+    <mergeCell ref="F6:O6"/>
+    <mergeCell ref="F7:O7"/>
+    <mergeCell ref="F12:O12"/>
+    <mergeCell ref="F8:O8"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2014,12 +2087,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Документ" ma:contentTypeID="0x010100EE0BF2D0F7DB87478EC6A86FB2228652" ma:contentTypeVersion="0" ma:contentTypeDescription="Создание документа." ma:contentTypeScope="" ma:versionID="6f37d12a6793316348e7f13d94897d83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="555e4f5434b0d6e16c19fe76cb398492">
     <xsd:element name="properties">
@@ -2133,6 +2200,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2143,21 +2216,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CF6FB7A-5EC0-4925-A25F-182A055EEC56}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF8F64BF-DA4F-4AD2-B9ED-9C10B5D873A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2173,6 +2231,21 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CF6FB7A-5EC0-4925-A25F-182A055EEC56}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{554579C4-AB49-4DF2-AFE6-C519C8775843}">
   <ds:schemaRefs>

</xml_diff>